<commit_message>
Updated Donor list Co-authored-by: Sang Ho Kwon
</commit_message>
<xml_diff>
--- a/code/xenium_panel_design/Xenium_DonorList.xlsx
+++ b/code/xenium_panel_design/Xenium_DonorList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanghokwon/Desktop/Lab/PNN_SCZ_Xenium/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bguo6/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8266FFB0-3490-BD43-9465-D151C63B4033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1912F31D-34C0-0546-BA57-0469F8F2E103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2700" yWindow="500" windowWidth="27640" windowHeight="16940" xr2:uid="{25845424-8B02-F84F-BB26-F457D7C6EFB0}"/>
+    <workbookView xWindow="2700" yWindow="500" windowWidth="27640" windowHeight="13900" xr2:uid="{25845424-8B02-F84F-BB26-F457D7C6EFB0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>NTC</t>
   </si>
@@ -105,7 +105,16 @@
     <t>ReadMe - Sheet2 has labels for each column</t>
   </si>
   <si>
-    <t>ReadMe - Sheet has NO labels for each column</t>
+    <t>Br6032</t>
+  </si>
+  <si>
+    <t>Br5436</t>
+  </si>
+  <si>
+    <t>Br5931</t>
+  </si>
+  <si>
+    <t>Br6389</t>
   </si>
 </sst>
 </file>
@@ -495,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2EEE142-CF94-B544-B871-40B04809725E}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,18 +515,15 @@
     <col min="4" max="4" width="37.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -525,7 +531,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -533,7 +539,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -541,7 +547,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -549,7 +555,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -557,7 +563,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>14</v>
       </c>
@@ -565,7 +571,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -573,7 +579,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -581,10 +587,28 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>